<commit_message>
Added Website Category and changed sequence numbers
Added Website Category and changed sequence numbers
</commit_message>
<xml_diff>
--- a/Documentation/Metrics fields and sequence number.xlsx
+++ b/Documentation/Metrics fields and sequence number.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centurylink-my.sharepoint.com/personal/billy_bennett_lumen_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centurylink-my.sharepoint.com/personal/billy_bennett_lumen_com/Documents/Documents/GitHub/HSORehdMetrics/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{3625347A-3CF6-4F46-9559-FF7A0CECC107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC4B0456-4C35-4780-832A-FF548A3FCF42}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{37FC37B3-BAA5-4352-A6BF-C4578865D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41D93BA0-2CD4-4CD9-B778-E88CE14CFBC3}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B754616-214D-4C02-8CFF-EFF6D36CED80}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="146">
   <si>
     <t>Category</t>
   </si>
@@ -466,6 +466,12 @@
   </si>
   <si>
     <t xml:space="preserve">Badges shipped </t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Website views</t>
   </si>
 </sst>
 </file>
@@ -730,9 +736,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,14 +771,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -785,12 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -804,7 +798,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1122,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66A4A06-3F38-46D9-B8DB-D4324A9B592B}">
-  <dimension ref="A1:X126"/>
+  <dimension ref="A1:X127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q124" sqref="Q124"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,13 +1200,13 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>100000</v>
       </c>
       <c r="D2" s="3">
@@ -1235,11 +1241,11 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>100100</v>
       </c>
       <c r="D3" s="3">
@@ -1274,11 +1280,11 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>100200</v>
       </c>
       <c r="D4" s="3">
@@ -1313,11 +1319,11 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>100300</v>
       </c>
       <c r="D5" s="10">
@@ -1378,13 +1384,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>100400</v>
       </c>
       <c r="D6" s="3">
@@ -1419,11 +1425,11 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>100500</v>
       </c>
       <c r="D7" s="3">
@@ -1458,11 +1464,11 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>100600</v>
       </c>
       <c r="D8" s="3">
@@ -1497,11 +1503,11 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>100700</v>
       </c>
       <c r="D9" s="10">
@@ -1562,13 +1568,13 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>100800</v>
       </c>
       <c r="D10" s="10">
@@ -1629,11 +1635,11 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>100900</v>
       </c>
       <c r="D11" s="10">
@@ -1694,11 +1700,11 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>101000</v>
       </c>
       <c r="D12" s="10">
@@ -1759,11 +1765,11 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>101100</v>
       </c>
       <c r="D13" s="10">
@@ -1824,13 +1830,13 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>101200</v>
       </c>
       <c r="D14" s="3">
@@ -1865,11 +1871,11 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <v>101300</v>
       </c>
       <c r="D15" s="3">
@@ -1904,11 +1910,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <v>101400</v>
       </c>
       <c r="D16" s="3">
@@ -1943,11 +1949,11 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>101500</v>
       </c>
       <c r="D17" s="10">
@@ -2008,13 +2014,13 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>101600</v>
       </c>
       <c r="D18" s="3">
@@ -2049,11 +2055,11 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>101700</v>
       </c>
       <c r="D19" s="3">
@@ -2088,11 +2094,11 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <v>101800</v>
       </c>
       <c r="D20" s="3">
@@ -2127,11 +2133,11 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="13">
         <v>101900</v>
       </c>
       <c r="D21" s="3">
@@ -2166,11 +2172,11 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>102000</v>
       </c>
       <c r="D22" s="3">
@@ -2205,11 +2211,11 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>102100</v>
       </c>
       <c r="D23" s="10">
@@ -2270,13 +2276,13 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="31" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="13">
         <v>102200</v>
       </c>
       <c r="D24" s="3">
@@ -2311,11 +2317,11 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="13">
         <v>102300</v>
       </c>
       <c r="D25" s="3">
@@ -2350,11 +2356,11 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="13">
         <v>102400</v>
       </c>
       <c r="D26" s="3">
@@ -2389,11 +2395,11 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="13">
         <v>102500</v>
       </c>
       <c r="D27" s="3">
@@ -2428,11 +2434,11 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="13">
         <v>102600</v>
       </c>
       <c r="D28" s="3">
@@ -2467,11 +2473,11 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="13">
         <v>102700</v>
       </c>
       <c r="D29" s="3">
@@ -2506,11 +2512,11 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="13">
         <v>102800</v>
       </c>
       <c r="D30" s="3">
@@ -2545,11 +2551,11 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="13">
         <v>102900</v>
       </c>
       <c r="D31" s="10">
@@ -2610,13 +2616,13 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="13">
         <v>103000</v>
       </c>
       <c r="D32" s="3">
@@ -2651,11 +2657,11 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="13">
         <v>103100</v>
       </c>
       <c r="D33" s="3">
@@ -2690,11 +2696,11 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="13">
         <v>103200</v>
       </c>
       <c r="D34" s="3">
@@ -2729,11 +2735,11 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="13">
         <v>103300</v>
       </c>
       <c r="D35" s="3">
@@ -2768,11 +2774,11 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="13">
         <v>103400</v>
       </c>
       <c r="D36" s="3">
@@ -2807,13 +2813,13 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="13">
         <v>103500</v>
       </c>
       <c r="D37" s="3">
@@ -2848,11 +2854,11 @@
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="13">
         <v>103600</v>
       </c>
       <c r="D38" s="3">
@@ -2887,11 +2893,11 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="13">
         <v>103700</v>
       </c>
       <c r="D39" s="3">
@@ -2926,11 +2932,11 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="13">
         <v>103800</v>
       </c>
       <c r="D40" s="3">
@@ -2965,11 +2971,11 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="14">
         <v>103900</v>
       </c>
       <c r="D41" s="3">
@@ -3004,13 +3010,13 @@
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="30" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="13">
         <v>104000</v>
       </c>
       <c r="D42" s="10">
@@ -3072,11 +3078,11 @@
       <c r="S42" s="12"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="13">
         <v>104100</v>
       </c>
       <c r="D43" s="10">
@@ -3137,66 +3143,66 @@
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="13">
         <v>104200</v>
       </c>
-      <c r="D44" s="18">
+      <c r="D44" s="17">
         <f>SUM(D43/D42)</f>
         <v>-4.6779417056495142E-3</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="17">
         <f t="shared" ref="E44:Q44" si="23">SUM(E43/E42)</f>
         <v>-8.8945362134688691E-3</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="17">
         <f t="shared" si="23"/>
         <v>-4.7410649161196208E-3</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="17">
         <f t="shared" si="23"/>
         <v>-1.8268176835951771E-3</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H44" s="17">
         <f t="shared" si="23"/>
         <v>-4.0352164343360232E-3</v>
       </c>
-      <c r="I44" s="18" t="e">
+      <c r="I44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J44" s="18" t="e">
+      <c r="J44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K44" s="18" t="e">
+      <c r="K44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L44" s="18" t="e">
+      <c r="L44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M44" s="18" t="e">
+      <c r="M44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N44" s="18" t="e">
+      <c r="N44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O44" s="18" t="e">
+      <c r="O44" s="17" t="e">
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P44" s="18">
+      <c r="P44" s="17">
         <f t="shared" si="23"/>
         <v>-4.8404119809295045E-3</v>
       </c>
-      <c r="Q44" s="18">
+      <c r="Q44" s="17">
         <f t="shared" si="23"/>
         <v>-4.9135577797998183E-3</v>
       </c>
@@ -3205,13 +3211,13 @@
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="30" t="s">
         <v>32</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="13">
         <v>104300</v>
       </c>
       <c r="D45" s="10">
@@ -3272,11 +3278,11 @@
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="13">
         <v>104400</v>
       </c>
       <c r="D46" s="10">
@@ -3337,66 +3343,66 @@
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="13">
         <v>104500</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D47" s="17">
         <f>SUM(D46/D45)</f>
         <v>-1.812688821752266E-2</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="17">
         <f t="shared" ref="E47:Q47" si="27">SUM(E46/E45)</f>
         <v>-1.5337423312883436E-2</v>
       </c>
-      <c r="F47" s="18">
+      <c r="F47" s="17">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="G47" s="18">
+      <c r="G47" s="17">
         <f t="shared" si="27"/>
         <v>-1.2944983818770227E-2</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="17">
         <f t="shared" si="27"/>
         <v>-1.3114754098360656E-2</v>
       </c>
-      <c r="I47" s="18" t="e">
+      <c r="I47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J47" s="18" t="e">
+      <c r="J47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K47" s="18" t="e">
+      <c r="K47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L47" s="18" t="e">
+      <c r="L47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M47" s="18" t="e">
+      <c r="M47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N47" s="18" t="e">
+      <c r="N47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O47" s="18" t="e">
+      <c r="O47" s="17" t="e">
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P47" s="18">
+      <c r="P47" s="17">
         <f t="shared" si="27"/>
         <v>-1.1994949494949494E-2</v>
       </c>
-      <c r="Q47" s="18">
+      <c r="Q47" s="17">
         <f t="shared" si="27"/>
         <v>-1.2618296529968454E-2</v>
       </c>
@@ -3405,13 +3411,13 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="13">
         <v>104600</v>
       </c>
       <c r="D48" s="10">
@@ -3473,11 +3479,11 @@
       <c r="S48" s="12"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="13">
         <v>104700</v>
       </c>
       <c r="D49" s="10">
@@ -3538,66 +3544,66 @@
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="13">
         <v>104800</v>
       </c>
-      <c r="D50" s="18">
+      <c r="D50" s="17">
         <f>SUM(D49/D48)</f>
         <v>-1.8998272884283247E-2</v>
       </c>
-      <c r="E50" s="18">
+      <c r="E50" s="17">
         <f t="shared" ref="E50:Q50" si="31">SUM(E49/E48)</f>
         <v>3.4423407917383822E-3</v>
       </c>
-      <c r="F50" s="18">
+      <c r="F50" s="17">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="17">
         <f t="shared" si="31"/>
         <v>8.5324232081911266E-3</v>
       </c>
-      <c r="H50" s="18">
+      <c r="H50" s="17">
         <f t="shared" si="31"/>
         <v>1.7035775127768314E-3</v>
       </c>
-      <c r="I50" s="18" t="e">
+      <c r="I50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J50" s="18" t="e">
+      <c r="J50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K50" s="18" t="e">
+      <c r="K50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L50" s="18" t="e">
+      <c r="L50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M50" s="18" t="e">
+      <c r="M50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N50" s="18" t="e">
+      <c r="N50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O50" s="18" t="e">
+      <c r="O50" s="17" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P50" s="18">
+      <c r="P50" s="17">
         <f t="shared" si="31"/>
         <v>-1.0295126973232671E-3</v>
       </c>
-      <c r="Q50" s="18">
+      <c r="Q50" s="17">
         <f t="shared" si="31"/>
         <v>-1.7152658662092624E-3</v>
       </c>
@@ -3606,13 +3612,13 @@
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="30" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="13">
         <v>104900</v>
       </c>
       <c r="D51" s="10">
@@ -3673,11 +3679,11 @@
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="13">
         <v>105000</v>
       </c>
       <c r="D52" s="10">
@@ -3738,66 +3744,66 @@
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="13">
         <v>105100</v>
       </c>
-      <c r="D53" s="18">
+      <c r="D53" s="17">
         <f>SUM(D52/D51)</f>
         <v>-6.6481137909709335E-3</v>
       </c>
-      <c r="E53" s="18">
+      <c r="E53" s="17">
         <f t="shared" ref="E53:Q53" si="35">SUM(E52/E51)</f>
         <v>-8.1047381546134663E-3</v>
       </c>
-      <c r="F53" s="18">
+      <c r="F53" s="17">
         <f t="shared" si="35"/>
         <v>-4.0765130134838507E-3</v>
       </c>
-      <c r="G53" s="18">
+      <c r="G53" s="17">
         <f t="shared" si="35"/>
         <v>-1.4130946773433821E-3</v>
       </c>
-      <c r="H53" s="18">
+      <c r="H53" s="17">
         <f t="shared" si="35"/>
         <v>-3.9407313997477933E-3</v>
       </c>
-      <c r="I53" s="18" t="e">
+      <c r="I53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J53" s="18" t="e">
+      <c r="J53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K53" s="18" t="e">
+      <c r="K53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L53" s="18" t="e">
+      <c r="L53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M53" s="18" t="e">
+      <c r="M53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N53" s="18" t="e">
+      <c r="N53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O53" s="18" t="e">
+      <c r="O53" s="17" t="e">
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P53" s="18">
+      <c r="P53" s="17">
         <f t="shared" si="35"/>
         <v>-4.8475371383893667E-3</v>
       </c>
-      <c r="Q53" s="18">
+      <c r="Q53" s="17">
         <f t="shared" si="35"/>
         <v>-4.8475371383893667E-3</v>
       </c>
@@ -3806,13 +3812,13 @@
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="31" t="s">
         <v>47</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="13">
         <v>105200</v>
       </c>
       <c r="D54" s="3">
@@ -3847,11 +3853,11 @@
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="34"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="13">
         <v>105300</v>
       </c>
       <c r="D55" s="3">
@@ -3886,11 +3892,11 @@
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="34"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="16">
+      <c r="C56" s="15">
         <v>105400</v>
       </c>
       <c r="D56" s="3">
@@ -3899,7 +3905,7 @@
       <c r="E56" s="3">
         <v>2.44</v>
       </c>
-      <c r="F56" s="19">
+      <c r="F56" s="18">
         <v>2.2999999999999998</v>
       </c>
       <c r="G56" s="3">
@@ -3925,11 +3931,11 @@
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="34"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="13">
         <v>105500</v>
       </c>
       <c r="D57" s="3">
@@ -3964,11 +3970,11 @@
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C58" s="13">
         <v>105600</v>
       </c>
       <c r="D58" s="3">
@@ -4003,11 +4009,11 @@
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="14">
+      <c r="C59" s="13">
         <v>105700</v>
       </c>
       <c r="D59" s="3">
@@ -4042,11 +4048,11 @@
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="34"/>
+      <c r="A60" s="32"/>
       <c r="B60" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="14">
+      <c r="C60" s="13">
         <v>105800</v>
       </c>
       <c r="D60" s="3">
@@ -4081,11 +4087,11 @@
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="34"/>
+      <c r="A61" s="32"/>
       <c r="B61" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="13">
         <v>105900</v>
       </c>
       <c r="D61" s="3">
@@ -4120,13 +4126,13 @@
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="33" t="s">
+      <c r="A62" s="31" t="s">
         <v>56</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="14">
+      <c r="C62" s="13">
         <v>106000</v>
       </c>
       <c r="D62" s="3">
@@ -4161,11 +4167,11 @@
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
+      <c r="A63" s="32"/>
       <c r="B63" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="13">
         <v>106100</v>
       </c>
       <c r="D63" s="3">
@@ -4200,11 +4206,11 @@
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C64" s="13">
         <v>106200</v>
       </c>
       <c r="D64" s="3">
@@ -4239,11 +4245,11 @@
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+      <c r="A65" s="32"/>
       <c r="B65" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C65" s="13">
         <v>106300</v>
       </c>
       <c r="D65" s="3">
@@ -4278,11 +4284,11 @@
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+      <c r="A66" s="37"/>
       <c r="B66" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66" s="13">
         <v>106400</v>
       </c>
       <c r="D66" s="10">
@@ -4343,13 +4349,13 @@
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="13">
         <v>106500</v>
       </c>
       <c r="D67" s="3">
@@ -4384,11 +4390,11 @@
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="32"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="14">
+      <c r="C68" s="13">
         <v>106600</v>
       </c>
       <c r="D68" s="3">
@@ -4423,11 +4429,11 @@
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C69" s="14">
+      <c r="C69" s="13">
         <v>106700</v>
       </c>
       <c r="D69" s="3">
@@ -4462,11 +4468,11 @@
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="14">
+      <c r="C70" s="13">
         <v>106800</v>
       </c>
       <c r="D70" s="3">
@@ -4501,11 +4507,11 @@
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C71" s="14">
+      <c r="C71" s="13">
         <v>106900</v>
       </c>
       <c r="D71" s="3">
@@ -4540,11 +4546,11 @@
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="32"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="14">
+      <c r="C72" s="13">
         <v>107000</v>
       </c>
       <c r="D72" s="10">
@@ -4605,11 +4611,11 @@
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="32"/>
+      <c r="A73" s="30"/>
       <c r="B73" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C73" s="14">
+      <c r="C73" s="13">
         <v>107100</v>
       </c>
       <c r="D73" s="3">
@@ -4644,11 +4650,11 @@
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="32"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="14">
+      <c r="C74" s="13">
         <v>107200</v>
       </c>
       <c r="D74" s="10">
@@ -4713,11 +4719,11 @@
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
+      <c r="A75" s="30"/>
       <c r="B75" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="14">
+      <c r="C75" s="13">
         <v>107300</v>
       </c>
       <c r="D75" s="3">
@@ -4752,11 +4758,11 @@
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" s="32"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C76" s="14">
+      <c r="C76" s="13">
         <v>107400</v>
       </c>
       <c r="D76" s="10">
@@ -4820,13 +4826,13 @@
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="32" t="s">
+      <c r="A77" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="14">
+      <c r="C77" s="13">
         <v>107500</v>
       </c>
       <c r="D77" s="3">
@@ -4861,11 +4867,11 @@
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" s="32"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="14">
+      <c r="C78" s="13">
         <v>107600</v>
       </c>
       <c r="D78" s="3">
@@ -4900,11 +4906,11 @@
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A79" s="32"/>
+      <c r="A79" s="30"/>
       <c r="B79" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="14">
+      <c r="C79" s="13">
         <v>107700</v>
       </c>
       <c r="D79" s="10">
@@ -4965,11 +4971,11 @@
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="14">
+      <c r="C80" s="13">
         <v>107800</v>
       </c>
       <c r="D80" s="3">
@@ -5004,11 +5010,11 @@
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A81" s="32"/>
+      <c r="A81" s="30"/>
       <c r="B81" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="14">
+      <c r="C81" s="13">
         <v>107900</v>
       </c>
       <c r="D81" s="3">
@@ -5043,11 +5049,11 @@
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="32"/>
+      <c r="A82" s="30"/>
       <c r="B82" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="14">
+      <c r="C82" s="13">
         <v>108000</v>
       </c>
       <c r="D82" s="3">
@@ -5082,11 +5088,11 @@
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A83" s="32"/>
+      <c r="A83" s="30"/>
       <c r="B83" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="14">
+      <c r="C83" s="13">
         <v>108100</v>
       </c>
       <c r="D83" s="3">
@@ -5121,11 +5127,11 @@
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A84" s="32"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="14">
+      <c r="C84" s="13">
         <v>108200</v>
       </c>
       <c r="D84" s="10">
@@ -5189,11 +5195,11 @@
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="32"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="14">
+      <c r="C85" s="13">
         <v>108300</v>
       </c>
       <c r="D85" s="3">
@@ -5224,13 +5230,13 @@
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="33" t="s">
+      <c r="A86" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C86" s="14">
+      <c r="C86" s="13">
         <v>108400</v>
       </c>
       <c r="D86" s="3">
@@ -5261,11 +5267,11 @@
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A87" s="34"/>
+      <c r="A87" s="32"/>
       <c r="B87" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C87" s="14">
+      <c r="C87" s="13">
         <v>108500</v>
       </c>
       <c r="D87" s="3">
@@ -5296,11 +5302,11 @@
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+      <c r="A88" s="32"/>
       <c r="B88" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C88" s="14">
+      <c r="C88" s="13">
         <v>108600</v>
       </c>
       <c r="D88" s="3">
@@ -5331,11 +5337,11 @@
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A89" s="35"/>
+      <c r="A89" s="37"/>
       <c r="B89" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C89" s="14">
+      <c r="C89" s="13">
         <v>108700</v>
       </c>
       <c r="D89" s="10">
@@ -5396,13 +5402,13 @@
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A90" s="41" t="s">
+      <c r="A90" s="38" t="s">
         <v>83</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C90" s="14">
+      <c r="C90" s="13">
         <v>108800</v>
       </c>
       <c r="D90" s="3">
@@ -5437,11 +5443,11 @@
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A91" s="41"/>
+      <c r="A91" s="38"/>
       <c r="B91" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="14">
+      <c r="C91" s="13">
         <v>108900</v>
       </c>
       <c r="D91" s="3">
@@ -5476,11 +5482,11 @@
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A92" s="41"/>
+      <c r="A92" s="38"/>
       <c r="B92" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="14">
+      <c r="C92" s="13">
         <v>109000</v>
       </c>
       <c r="D92" s="11">
@@ -5542,14 +5548,14 @@
       <c r="T92" t="s">
         <v>100</v>
       </c>
-      <c r="V92" s="25"/>
+      <c r="V92" s="24"/>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="39"/>
       <c r="B93" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C93" s="14">
+      <c r="C93" s="13">
         <v>109100</v>
       </c>
       <c r="D93" s="3">
@@ -5578,7 +5584,7 @@
         <f t="shared" ref="P93" si="56">SUM(D93+E93+F93+G93+H93+I93+J93+K93+L93+M93+N93+O93+O93)</f>
         <v>23.66</v>
       </c>
-      <c r="Q93" s="27">
+      <c r="Q93" s="26">
         <v>4.7300000000000004</v>
       </c>
       <c r="T93" t="s">
@@ -5586,11 +5592,11 @@
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="39"/>
       <c r="B94" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C94" s="14">
+      <c r="C94" s="13">
         <v>109200</v>
       </c>
       <c r="D94" s="3">
@@ -5616,10 +5622,10 @@
       <c r="N94" s="3"/>
       <c r="O94" s="3"/>
       <c r="P94" s="3">
-        <f t="shared" ref="P94:P105" si="57">SUM(D94+E94+F94+G94+H94+I94+J94+K94+L94+M94+N94+O94+O94)</f>
+        <f t="shared" ref="P94:P106" si="57">SUM(D94+E94+F94+G94+H94+I94+J94+K94+L94+M94+N94+O94+O94)</f>
         <v>47.96</v>
       </c>
-      <c r="Q94" s="27">
+      <c r="Q94" s="26">
         <f t="shared" ref="Q94:Q96" si="58">ROUND(SUM(P94/5),0)</f>
         <v>10</v>
       </c>
@@ -5628,11 +5634,11 @@
       </c>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
+      <c r="A95" s="16"/>
       <c r="B95" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C95" s="14">
+      <c r="C95" s="13">
         <v>109300</v>
       </c>
       <c r="D95" s="3">
@@ -5667,11 +5673,11 @@
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
+      <c r="A96" s="16"/>
       <c r="B96" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C96" s="14">
+      <c r="C96" s="13">
         <v>109400</v>
       </c>
       <c r="D96" s="3">
@@ -5706,11 +5712,11 @@
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
+      <c r="A97" s="16"/>
       <c r="B97" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C97" s="14">
+      <c r="C97" s="13">
         <v>109500</v>
       </c>
       <c r="D97" s="10" t="e">
@@ -5774,11 +5780,11 @@
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
+      <c r="A98" s="16"/>
       <c r="B98" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C98" s="14">
+      <c r="C98" s="13">
         <v>109600</v>
       </c>
       <c r="D98" s="3">
@@ -5804,7 +5810,7 @@
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
       <c r="P98" s="3">
-        <f t="shared" ref="P98:P101" si="60">SUM(D98+E98+F98+G98+H98+I98+J98+K98+L98+M98+N98+O98+O98)</f>
+        <f t="shared" ref="P98:P102" si="60">SUM(D98+E98+F98+G98+H98+I98+J98+K98+L98+M98+N98+O98+O98)</f>
         <v>14.899999999999999</v>
       </c>
       <c r="Q98" s="3">
@@ -5815,11 +5821,11 @@
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A99" s="13"/>
+      <c r="A99" s="16"/>
       <c r="B99" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C99" s="14">
+      <c r="C99" s="13">
         <v>109700</v>
       </c>
       <c r="D99" s="3">
@@ -5845,7 +5851,7 @@
       <c r="N99" s="3"/>
       <c r="O99" s="3"/>
       <c r="P99" s="3">
-        <f t="shared" si="60"/>
+        <f t="shared" ref="P99" si="61">SUM(D99+E99+F99+G99+H99+I99+J99+K99+L99+M99+N99+O99+O99)</f>
         <v>29.32</v>
       </c>
       <c r="Q99" s="3">
@@ -5856,30 +5862,20 @@
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A100" s="29" t="s">
-        <v>84</v>
+      <c r="A100" s="28" t="s">
+        <v>144</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C100" s="14">
+        <v>145</v>
+      </c>
+      <c r="C100" s="13">
         <v>109800</v>
       </c>
-      <c r="D100" s="3">
-        <v>74777</v>
-      </c>
-      <c r="E100" s="3">
-        <v>77997</v>
-      </c>
-      <c r="F100" s="3">
-        <v>77443</v>
-      </c>
-      <c r="G100" s="3">
-        <v>79826</v>
-      </c>
-      <c r="H100" s="3">
-        <v>75304</v>
-      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
@@ -5887,31 +5883,33 @@
       <c r="M100" s="3"/>
       <c r="N100" s="3"/>
       <c r="O100" s="3"/>
-      <c r="P100" s="3">
-        <f t="shared" si="60"/>
-        <v>385347</v>
-      </c>
-      <c r="Q100" s="3">
-        <f t="shared" ref="Q100" si="61">ROUND(SUM(P100/5),0)</f>
-        <v>77069</v>
-      </c>
+      <c r="P100" s="3"/>
+      <c r="Q100" s="3"/>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="39" t="s">
+        <v>84</v>
+      </c>
       <c r="B101" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C101" s="14">
-        <v>109900</v>
-      </c>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="C101" s="13">
+        <v>110000</v>
+      </c>
+      <c r="D101" s="3">
+        <v>74777</v>
+      </c>
+      <c r="E101" s="3">
+        <v>77997</v>
+      </c>
+      <c r="F101" s="3">
+        <v>77443</v>
+      </c>
       <c r="G101" s="3">
-        <v>98.62</v>
+        <v>79826</v>
       </c>
       <c r="H101" s="3">
-        <v>99.01</v>
+        <v>75304</v>
       </c>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
@@ -5922,115 +5920,109 @@
       <c r="O101" s="3"/>
       <c r="P101" s="3">
         <f t="shared" si="60"/>
+        <v>385347</v>
+      </c>
+      <c r="Q101" s="3">
+        <f t="shared" ref="Q101" si="62">ROUND(SUM(P101/5),0)</f>
+        <v>77069</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A102" s="40"/>
+      <c r="B102" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C102" s="13">
+        <v>110100</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3">
+        <v>98.62</v>
+      </c>
+      <c r="H102" s="3">
+        <v>99.01</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+      <c r="P102" s="3">
+        <f t="shared" si="60"/>
         <v>197.63</v>
       </c>
-      <c r="Q101" s="3">
+      <c r="Q102" s="3">
         <v>98.81</v>
       </c>
-      <c r="T101" t="s">
+      <c r="T102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="31"/>
-      <c r="B102" s="7" t="s">
+    <row r="103" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A103" s="41"/>
+      <c r="B103" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C102" s="14">
-        <v>110000</v>
-      </c>
-      <c r="D102" s="28">
+      <c r="C103" s="13">
+        <v>110200</v>
+      </c>
+      <c r="D103" s="27">
         <v>98.35</v>
       </c>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28" t="s">
+      <c r="E103" s="27"/>
+      <c r="F103" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="G102" s="28">
+      <c r="G103" s="27">
         <v>52.54</v>
       </c>
-      <c r="H102" s="28"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
-      <c r="K102" s="28"/>
-      <c r="L102" s="28"/>
-      <c r="M102" s="28"/>
-      <c r="N102" s="28"/>
-      <c r="O102" s="28"/>
-      <c r="P102" s="28">
-        <f>SUM(D102:O102)</f>
+      <c r="H103" s="27"/>
+      <c r="I103" s="27"/>
+      <c r="J103" s="27"/>
+      <c r="K103" s="27"/>
+      <c r="L103" s="27"/>
+      <c r="M103" s="27"/>
+      <c r="N103" s="27"/>
+      <c r="O103" s="27"/>
+      <c r="P103" s="27">
+        <f>SUM(D103:O103)</f>
         <v>150.88999999999999</v>
       </c>
-      <c r="Q102" s="3">
+      <c r="Q103" s="3">
         <v>75.44</v>
       </c>
-      <c r="T102" s="26" t="s">
+      <c r="T103" s="25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A104" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C103" s="14">
-        <v>110100</v>
-      </c>
-      <c r="D103" s="3">
+      <c r="C104" s="13">
+        <v>110300</v>
+      </c>
+      <c r="D104" s="3">
         <v>32</v>
       </c>
-      <c r="E103" s="3">
+      <c r="E104" s="3">
         <v>35</v>
       </c>
-      <c r="F103" s="3">
+      <c r="F104" s="3">
         <v>35</v>
       </c>
-      <c r="G103" s="3">
+      <c r="G104" s="3">
         <v>35</v>
       </c>
-      <c r="H103" s="3">
+      <c r="H104" s="3">
         <v>35</v>
-      </c>
-      <c r="I103" s="3"/>
-      <c r="J103" s="3"/>
-      <c r="K103" s="3"/>
-      <c r="L103" s="3"/>
-      <c r="M103" s="3"/>
-      <c r="N103" s="3"/>
-      <c r="O103" s="3"/>
-      <c r="P103" s="3">
-        <f t="shared" si="57"/>
-        <v>172</v>
-      </c>
-      <c r="Q103" s="3">
-        <f t="shared" ref="Q103" si="62">ROUND(SUM(P103/5),0)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
-      <c r="B104" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C104" s="14">
-        <v>110200</v>
-      </c>
-      <c r="D104" s="3">
-        <v>3</v>
-      </c>
-      <c r="E104" s="3">
-        <v>3</v>
-      </c>
-      <c r="F104" s="3">
-        <v>3</v>
-      </c>
-      <c r="G104" s="3">
-        <v>3</v>
-      </c>
-      <c r="H104" s="3">
-        <v>3</v>
       </c>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
@@ -6041,38 +6033,35 @@
       <c r="O104" s="3"/>
       <c r="P104" s="3">
         <f t="shared" si="57"/>
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="Q104" s="3">
-        <f t="shared" ref="Q104:Q105" si="63">ROUND(SUM(P104/5),0)</f>
+        <f t="shared" ref="Q104" si="63">ROUND(SUM(P104/5),0)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A105" s="30"/>
+      <c r="B105" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105" s="13">
+        <v>110400</v>
+      </c>
+      <c r="D105" s="3">
         <v>3</v>
       </c>
-      <c r="T104" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A105" s="32"/>
-      <c r="B105" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C105" s="14">
-        <v>110300</v>
-      </c>
-      <c r="D105" s="3">
-        <v>1</v>
-      </c>
       <c r="E105" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F105" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G105" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H105" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
@@ -6083,141 +6072,144 @@
       <c r="O105" s="3"/>
       <c r="P105" s="3">
         <f t="shared" si="57"/>
+        <v>15</v>
+      </c>
+      <c r="Q105" s="3">
+        <f t="shared" ref="Q105:Q106" si="64">ROUND(SUM(P105/5),0)</f>
+        <v>3</v>
+      </c>
+      <c r="T105" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A106" s="30"/>
+      <c r="B106" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C106" s="13">
+        <v>110500</v>
+      </c>
+      <c r="D106" s="3">
+        <v>1</v>
+      </c>
+      <c r="E106" s="3">
+        <v>1</v>
+      </c>
+      <c r="F106" s="3">
+        <v>1</v>
+      </c>
+      <c r="G106" s="3">
+        <v>1</v>
+      </c>
+      <c r="H106" s="3">
+        <v>1</v>
+      </c>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3">
+        <f t="shared" si="57"/>
         <v>5</v>
       </c>
-      <c r="Q105" s="3">
-        <f t="shared" si="63"/>
+      <c r="Q106" s="3">
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A106" s="32"/>
-      <c r="B106" s="7" t="s">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A107" s="30"/>
+      <c r="B107" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C106" s="14">
-        <v>110400</v>
-      </c>
-      <c r="D106" s="10">
-        <f>SUM(D103:D105)</f>
+      <c r="C107" s="13">
+        <v>110600</v>
+      </c>
+      <c r="D107" s="10">
+        <f>SUM(D104:D106)</f>
         <v>36</v>
       </c>
-      <c r="E106" s="10">
-        <f t="shared" ref="E106:P106" si="64">SUM(E103:E105)</f>
+      <c r="E107" s="10">
+        <f t="shared" ref="E107:P107" si="65">SUM(E104:E106)</f>
         <v>39</v>
       </c>
-      <c r="F106" s="10">
-        <f t="shared" si="64"/>
+      <c r="F107" s="10">
+        <f t="shared" si="65"/>
         <v>39</v>
       </c>
-      <c r="G106" s="10">
-        <f t="shared" si="64"/>
+      <c r="G107" s="10">
+        <f t="shared" si="65"/>
         <v>39</v>
       </c>
-      <c r="H106" s="10">
-        <f t="shared" si="64"/>
+      <c r="H107" s="10">
+        <f t="shared" si="65"/>
         <v>39</v>
       </c>
-      <c r="I106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="J106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="K106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="L106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="M106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="N106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="O106" s="10">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="P106" s="10">
-        <f t="shared" si="64"/>
+      <c r="I107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="J107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="K107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="L107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="M107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="N107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="O107" s="10">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="P107" s="10">
+        <f t="shared" si="65"/>
         <v>192</v>
       </c>
-      <c r="Q106" s="10">
-        <f>ROUND(SUM(P106/5),0)</f>
+      <c r="Q107" s="10">
+        <f>ROUND(SUM(P107/5),0)</f>
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A107" s="33" t="s">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A108" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B108" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C107" s="14">
-        <v>110500</v>
-      </c>
-      <c r="D107" s="3">
+      <c r="C108" s="13">
+        <v>110700</v>
+      </c>
+      <c r="D108" s="3">
         <v>2</v>
       </c>
-      <c r="E107" s="3">
+      <c r="E108" s="3">
         <v>5</v>
       </c>
-      <c r="F107" s="3">
+      <c r="F108" s="3">
         <v>7</v>
       </c>
-      <c r="G107" s="3">
+      <c r="G108" s="3">
         <v>21</v>
       </c>
-      <c r="H107" s="3">
+      <c r="H108" s="3">
         <v>2</v>
-      </c>
-      <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3">
-        <f t="shared" ref="P107:P116" si="65">SUM(D107+E107+F107+G107+H107+I107+J107+K107+L107+M107+N107+O107+O107)</f>
-        <v>37</v>
-      </c>
-      <c r="Q107" s="3">
-        <f t="shared" ref="Q107:Q116" si="66">ROUND(SUM(P107/5),0)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A108" s="35"/>
-      <c r="B108" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C108" s="14">
-        <v>110600</v>
-      </c>
-      <c r="D108" s="3">
-        <v>3</v>
-      </c>
-      <c r="E108" s="3">
-        <v>4</v>
-      </c>
-      <c r="F108" s="3">
-        <v>4</v>
-      </c>
-      <c r="G108" s="3">
-        <v>5</v>
-      </c>
-      <c r="H108" s="3">
-        <v>9</v>
       </c>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
@@ -6227,41 +6219,36 @@
       <c r="N108" s="3"/>
       <c r="O108" s="3"/>
       <c r="P108" s="3">
-        <f t="shared" si="65"/>
-        <v>25</v>
+        <f t="shared" ref="P108:P117" si="66">SUM(D108+E108+F108+G108+H108+I108+J108+K108+L108+M108+N108+O108+O108)</f>
+        <v>37</v>
       </c>
       <c r="Q108" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" ref="Q108:Q117" si="67">ROUND(SUM(P108/5),0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A109" s="37"/>
+      <c r="B109" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C109" s="13">
+        <v>110800</v>
+      </c>
+      <c r="D109" s="3">
+        <v>3</v>
+      </c>
+      <c r="E109" s="3">
+        <v>4</v>
+      </c>
+      <c r="F109" s="3">
+        <v>4</v>
+      </c>
+      <c r="G109" s="3">
         <v>5</v>
       </c>
-      <c r="T108" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A109" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C109" s="14">
-        <v>110700</v>
-      </c>
-      <c r="D109" s="3">
-        <v>32</v>
-      </c>
-      <c r="E109" s="3">
-        <v>40</v>
-      </c>
-      <c r="F109" s="3">
-        <v>38</v>
-      </c>
-      <c r="G109" s="3">
-        <v>47</v>
-      </c>
       <c r="H109" s="3">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
@@ -6271,287 +6258,292 @@
       <c r="N109" s="3"/>
       <c r="O109" s="3"/>
       <c r="P109" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
+        <v>25</v>
+      </c>
+      <c r="Q109" s="3">
+        <f t="shared" si="67"/>
+        <v>5</v>
+      </c>
+      <c r="T109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A110" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C110" s="13">
+        <v>110900</v>
+      </c>
+      <c r="D110" s="3">
+        <v>32</v>
+      </c>
+      <c r="E110" s="3">
+        <v>40</v>
+      </c>
+      <c r="F110" s="3">
+        <v>38</v>
+      </c>
+      <c r="G110" s="3">
+        <v>47</v>
+      </c>
+      <c r="H110" s="3">
+        <v>42</v>
+      </c>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="3"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="3"/>
+      <c r="P110" s="3">
+        <f t="shared" si="66"/>
         <v>199</v>
       </c>
-      <c r="Q109" s="3">
+      <c r="Q110" s="3">
+        <f t="shared" si="67"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="40"/>
+      <c r="B111" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" s="13">
+        <v>111000</v>
+      </c>
+      <c r="D111" s="27">
+        <v>5842</v>
+      </c>
+      <c r="E111" s="27">
+        <v>148</v>
+      </c>
+      <c r="F111" s="27">
+        <v>5874</v>
+      </c>
+      <c r="G111" s="27">
+        <v>6421</v>
+      </c>
+      <c r="H111" s="27">
+        <v>8421</v>
+      </c>
+      <c r="I111" s="27"/>
+      <c r="J111" s="27"/>
+      <c r="K111" s="27"/>
+      <c r="L111" s="27"/>
+      <c r="M111" s="27"/>
+      <c r="N111" s="27"/>
+      <c r="O111" s="27"/>
+      <c r="P111" s="27">
         <f t="shared" si="66"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="30"/>
-      <c r="B110" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C110" s="14">
-        <v>110800</v>
-      </c>
-      <c r="D110" s="28">
-        <v>5842</v>
-      </c>
-      <c r="E110" s="28">
-        <v>148</v>
-      </c>
-      <c r="F110" s="28">
-        <v>5874</v>
-      </c>
-      <c r="G110" s="28">
-        <v>6421</v>
-      </c>
-      <c r="H110" s="28">
-        <v>8421</v>
-      </c>
-      <c r="I110" s="28"/>
-      <c r="J110" s="28"/>
-      <c r="K110" s="28"/>
-      <c r="L110" s="28"/>
-      <c r="M110" s="28"/>
-      <c r="N110" s="28"/>
-      <c r="O110" s="28"/>
-      <c r="P110" s="28">
-        <f t="shared" si="65"/>
         <v>26706</v>
       </c>
-      <c r="Q110" s="28">
-        <f t="shared" si="66"/>
+      <c r="Q111" s="27">
+        <f t="shared" si="67"/>
         <v>5341</v>
-      </c>
-      <c r="T110" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="111" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
-      <c r="B111" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C111" s="14">
-        <v>110900</v>
-      </c>
-      <c r="D111" s="28">
-        <v>11500</v>
-      </c>
-      <c r="E111" s="28">
-        <v>1500</v>
-      </c>
-      <c r="F111" s="28">
-        <v>40000</v>
-      </c>
-      <c r="G111" s="28">
-        <v>15000</v>
-      </c>
-      <c r="H111" s="28">
-        <v>19000</v>
-      </c>
-      <c r="I111" s="28"/>
-      <c r="J111" s="28"/>
-      <c r="K111" s="28"/>
-      <c r="L111" s="28"/>
-      <c r="M111" s="28"/>
-      <c r="N111" s="28"/>
-      <c r="O111" s="28"/>
-      <c r="P111" s="28">
-        <f t="shared" si="65"/>
-        <v>87000</v>
-      </c>
-      <c r="Q111" s="28">
-        <f t="shared" si="66"/>
-        <v>17400</v>
       </c>
       <c r="T111" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="112" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
-      <c r="B112" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C112" s="14">
-        <v>111000</v>
-      </c>
-      <c r="D112" s="28">
-        <v>5000</v>
-      </c>
-      <c r="E112" s="28">
-        <v>5000</v>
-      </c>
-      <c r="F112" s="28">
-        <v>1000</v>
-      </c>
-      <c r="G112" s="28">
-        <v>2000</v>
-      </c>
-      <c r="H112" s="28">
-        <v>3000</v>
-      </c>
-      <c r="I112" s="28"/>
-      <c r="J112" s="28"/>
-      <c r="K112" s="28"/>
-      <c r="L112" s="28"/>
-      <c r="M112" s="28"/>
-      <c r="N112" s="28"/>
-      <c r="O112" s="28"/>
-      <c r="P112" s="28">
-        <f t="shared" si="65"/>
-        <v>16000</v>
-      </c>
-      <c r="Q112" s="28">
+      <c r="A112" s="40"/>
+      <c r="B112" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112" s="13">
+        <v>111100</v>
+      </c>
+      <c r="D112" s="27">
+        <v>11500</v>
+      </c>
+      <c r="E112" s="27">
+        <v>1500</v>
+      </c>
+      <c r="F112" s="27">
+        <v>40000</v>
+      </c>
+      <c r="G112" s="27">
+        <v>15000</v>
+      </c>
+      <c r="H112" s="27">
+        <v>19000</v>
+      </c>
+      <c r="I112" s="27"/>
+      <c r="J112" s="27"/>
+      <c r="K112" s="27"/>
+      <c r="L112" s="27"/>
+      <c r="M112" s="27"/>
+      <c r="N112" s="27"/>
+      <c r="O112" s="27"/>
+      <c r="P112" s="27">
         <f t="shared" si="66"/>
-        <v>3200</v>
+        <v>87000</v>
+      </c>
+      <c r="Q112" s="27">
+        <f t="shared" si="67"/>
+        <v>17400</v>
       </c>
       <c r="T112" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="113" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
-      <c r="B113" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C113" s="14">
-        <v>111100</v>
-      </c>
-      <c r="D113" s="28">
+      <c r="A113" s="40"/>
+      <c r="B113" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113" s="13">
+        <v>111200</v>
+      </c>
+      <c r="D113" s="27">
+        <v>5000</v>
+      </c>
+      <c r="E113" s="27">
+        <v>5000</v>
+      </c>
+      <c r="F113" s="27">
         <v>1000</v>
       </c>
-      <c r="E113" s="28">
-        <v>10000</v>
-      </c>
-      <c r="F113" s="28">
-        <v>15000</v>
-      </c>
-      <c r="G113" s="28">
-        <v>20000</v>
-      </c>
-      <c r="H113" s="28">
-        <v>15000</v>
-      </c>
-      <c r="I113" s="28"/>
-      <c r="J113" s="28"/>
-      <c r="K113" s="28"/>
-      <c r="L113" s="28"/>
-      <c r="M113" s="28"/>
-      <c r="N113" s="28"/>
-      <c r="O113" s="28"/>
-      <c r="P113" s="28">
-        <f t="shared" si="65"/>
-        <v>61000</v>
-      </c>
-      <c r="Q113" s="28">
+      <c r="G113" s="27">
+        <v>2000</v>
+      </c>
+      <c r="H113" s="27">
+        <v>3000</v>
+      </c>
+      <c r="I113" s="27"/>
+      <c r="J113" s="27"/>
+      <c r="K113" s="27"/>
+      <c r="L113" s="27"/>
+      <c r="M113" s="27"/>
+      <c r="N113" s="27"/>
+      <c r="O113" s="27"/>
+      <c r="P113" s="27">
         <f t="shared" si="66"/>
-        <v>12200</v>
+        <v>16000</v>
+      </c>
+      <c r="Q113" s="27">
+        <f t="shared" si="67"/>
+        <v>3200</v>
       </c>
       <c r="T113" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="114" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="31"/>
-      <c r="B114" s="20" t="s">
+      <c r="A114" s="40"/>
+      <c r="B114" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114" s="13">
+        <v>111300</v>
+      </c>
+      <c r="D114" s="27">
+        <v>1000</v>
+      </c>
+      <c r="E114" s="27">
+        <v>10000</v>
+      </c>
+      <c r="F114" s="27">
+        <v>15000</v>
+      </c>
+      <c r="G114" s="27">
+        <v>20000</v>
+      </c>
+      <c r="H114" s="27">
+        <v>15000</v>
+      </c>
+      <c r="I114" s="27"/>
+      <c r="J114" s="27"/>
+      <c r="K114" s="27"/>
+      <c r="L114" s="27"/>
+      <c r="M114" s="27"/>
+      <c r="N114" s="27"/>
+      <c r="O114" s="27"/>
+      <c r="P114" s="27">
+        <f t="shared" si="66"/>
+        <v>61000</v>
+      </c>
+      <c r="Q114" s="27">
+        <f t="shared" si="67"/>
+        <v>12200</v>
+      </c>
+      <c r="T114" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="41"/>
+      <c r="B115" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C114" s="14">
-        <v>111200</v>
-      </c>
-      <c r="D114" s="28">
+      <c r="C115" s="13">
+        <v>111400</v>
+      </c>
+      <c r="D115" s="27">
         <v>119542</v>
       </c>
-      <c r="E114" s="28">
+      <c r="E115" s="27">
         <v>154212</v>
       </c>
-      <c r="F114" s="28">
+      <c r="F115" s="27">
         <v>154154</v>
       </c>
-      <c r="G114" s="28">
+      <c r="G115" s="27">
         <v>142544</v>
       </c>
-      <c r="H114" s="28">
+      <c r="H115" s="27">
         <v>145411</v>
       </c>
-      <c r="I114" s="28"/>
-      <c r="J114" s="28"/>
-      <c r="K114" s="28"/>
-      <c r="L114" s="28"/>
-      <c r="M114" s="28"/>
-      <c r="N114" s="28"/>
-      <c r="O114" s="28"/>
-      <c r="P114" s="28">
-        <f t="shared" si="65"/>
+      <c r="I115" s="27"/>
+      <c r="J115" s="27"/>
+      <c r="K115" s="27"/>
+      <c r="L115" s="27"/>
+      <c r="M115" s="27"/>
+      <c r="N115" s="27"/>
+      <c r="O115" s="27"/>
+      <c r="P115" s="27">
+        <f t="shared" si="66"/>
         <v>715863</v>
       </c>
-      <c r="Q114" s="28">
-        <f t="shared" si="66"/>
+      <c r="Q115" s="27">
+        <f t="shared" si="67"/>
         <v>143173</v>
       </c>
-      <c r="T114" t="s">
+      <c r="T115" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A115" s="33" t="s">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A116" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="B115" s="7" t="s">
+      <c r="B116" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C115" s="14">
-        <v>111300</v>
-      </c>
-      <c r="D115" s="3">
+      <c r="C116" s="13">
+        <v>111500</v>
+      </c>
+      <c r="D116" s="3">
         <v>798</v>
       </c>
-      <c r="E115" s="3">
+      <c r="E116" s="3">
         <v>791</v>
       </c>
-      <c r="F115" s="3">
+      <c r="F116" s="3">
         <v>726</v>
       </c>
-      <c r="G115" s="3">
+      <c r="G116" s="3">
         <v>686</v>
       </c>
-      <c r="H115" s="3">
+      <c r="H116" s="3">
         <v>782</v>
-      </c>
-      <c r="I115" s="3"/>
-      <c r="J115" s="3"/>
-      <c r="K115" s="3"/>
-      <c r="L115" s="3"/>
-      <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
-      <c r="O115" s="3"/>
-      <c r="P115" s="3">
-        <f t="shared" si="65"/>
-        <v>3783</v>
-      </c>
-      <c r="Q115" s="3">
-        <f t="shared" si="66"/>
-        <v>757</v>
-      </c>
-    </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
-      <c r="B116" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C116" s="14">
-        <v>111400</v>
-      </c>
-      <c r="D116" s="3">
-        <v>445</v>
-      </c>
-      <c r="E116" s="3">
-        <v>439</v>
-      </c>
-      <c r="F116" s="3">
-        <v>446</v>
-      </c>
-      <c r="G116" s="3">
-        <v>395</v>
-      </c>
-      <c r="H116" s="3">
-        <v>440</v>
       </c>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
@@ -6561,138 +6553,142 @@
       <c r="N116" s="3"/>
       <c r="O116" s="3"/>
       <c r="P116" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
+        <v>3783</v>
+      </c>
+      <c r="Q116" s="3">
+        <f t="shared" si="67"/>
+        <v>757</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A117" s="32"/>
+      <c r="B117" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C117" s="13">
+        <v>111600</v>
+      </c>
+      <c r="D117" s="3">
+        <v>445</v>
+      </c>
+      <c r="E117" s="3">
+        <v>439</v>
+      </c>
+      <c r="F117" s="3">
+        <v>446</v>
+      </c>
+      <c r="G117" s="3">
+        <v>395</v>
+      </c>
+      <c r="H117" s="3">
+        <v>440</v>
+      </c>
+      <c r="I117" s="3"/>
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+      <c r="L117" s="3"/>
+      <c r="M117" s="3"/>
+      <c r="N117" s="3"/>
+      <c r="O117" s="3"/>
+      <c r="P117" s="3">
+        <f t="shared" si="66"/>
         <v>2165</v>
       </c>
-      <c r="Q116" s="3">
-        <f t="shared" si="66"/>
+      <c r="Q117" s="3">
+        <f t="shared" si="67"/>
         <v>433</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
-      <c r="B117" s="9" t="s">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A118" s="32"/>
+      <c r="B118" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C117" s="14">
-        <v>111500</v>
-      </c>
-      <c r="D117" s="10">
-        <f>SUM(D115:D116)</f>
+      <c r="C118" s="13">
+        <v>111700</v>
+      </c>
+      <c r="D118" s="10">
+        <f>SUM(D116:D117)</f>
         <v>1243</v>
       </c>
-      <c r="E117" s="10">
-        <f t="shared" ref="E117:Q117" si="67">SUM(E115:E116)</f>
+      <c r="E118" s="10">
+        <f t="shared" ref="E118:Q118" si="68">SUM(E116:E117)</f>
         <v>1230</v>
       </c>
-      <c r="F117" s="10">
-        <f t="shared" si="67"/>
+      <c r="F118" s="10">
+        <f t="shared" si="68"/>
         <v>1172</v>
       </c>
-      <c r="G117" s="10">
-        <f t="shared" si="67"/>
+      <c r="G118" s="10">
+        <f t="shared" si="68"/>
         <v>1081</v>
       </c>
-      <c r="H117" s="10">
-        <f t="shared" si="67"/>
+      <c r="H118" s="10">
+        <f t="shared" si="68"/>
         <v>1222</v>
       </c>
-      <c r="I117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="J117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="K117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="L117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="M117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="N117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="O117" s="10">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="P117" s="10">
-        <f t="shared" si="67"/>
+      <c r="I118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="J118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="K118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="L118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="M118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="N118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="O118" s="10">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="P118" s="10">
+        <f t="shared" si="68"/>
         <v>5948</v>
       </c>
-      <c r="Q117" s="10">
-        <f t="shared" si="67"/>
+      <c r="Q118" s="10">
+        <f t="shared" si="68"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A118" s="37"/>
-      <c r="B118" s="7" t="s">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A119" s="33"/>
+      <c r="B119" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C118" s="14">
-        <v>111600</v>
-      </c>
-      <c r="D118" s="3">
-        <v>0</v>
-      </c>
-      <c r="E118" s="3">
-        <v>0</v>
-      </c>
-      <c r="F118" s="3">
-        <v>0</v>
-      </c>
-      <c r="G118" s="3">
-        <v>0</v>
-      </c>
-      <c r="H118" s="3">
-        <v>0</v>
-      </c>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
-      <c r="L118" s="3"/>
-      <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
-      <c r="O118" s="3"/>
-      <c r="P118" s="3">
-        <f>SUM(D118+E118+F118+G118+H118+I118+J118+K118+L118+M118+N118+O118+O118)</f>
-        <v>0</v>
-      </c>
-      <c r="Q118" s="3">
-        <f t="shared" ref="Q118:Q126" si="68">ROUND(SUM(P118/5),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B119" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C119" s="14">
-        <v>111700</v>
-      </c>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
+      <c r="C119" s="13">
+        <v>111800</v>
+      </c>
+      <c r="D119" s="3">
+        <v>0</v>
+      </c>
+      <c r="E119" s="3">
+        <v>0</v>
+      </c>
+      <c r="F119" s="3">
+        <v>0</v>
+      </c>
+      <c r="G119" s="3">
+        <v>0</v>
+      </c>
       <c r="H119" s="3">
-        <v>2</v>
-      </c>
-      <c r="I119" s="3">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
@@ -6700,37 +6696,33 @@
       <c r="N119" s="3"/>
       <c r="O119" s="3"/>
       <c r="P119" s="3">
-        <f t="shared" ref="P119:P120" si="69">SUM(D119+E119+F119+G119+H119+I119+J119+K119+L119+M119+N119+O119+O119)</f>
-        <v>4</v>
+        <f>SUM(D119+E119+F119+G119+H119+I119+J119+K119+L119+M119+N119+O119+O119)</f>
+        <v>0</v>
       </c>
       <c r="Q119" s="3">
-        <f>ROUND(SUM(P119/2),0)</f>
-        <v>2</v>
-      </c>
-      <c r="T119" t="s">
-        <v>137</v>
-      </c>
-      <c r="U119" t="s">
-        <v>141</v>
+        <f t="shared" ref="Q119:Q124" si="69">ROUND(SUM(P119/5),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="39"/>
-      <c r="B120" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C120" s="14">
-        <v>111800</v>
+      <c r="A120" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B120" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C120" s="13">
+        <v>111900</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="I120" s="3">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
@@ -6739,12 +6731,12 @@
       <c r="N120" s="3"/>
       <c r="O120" s="3"/>
       <c r="P120" s="3">
-        <f t="shared" si="69"/>
-        <v>149</v>
+        <f t="shared" ref="P120:P121" si="70">SUM(D120+E120+F120+G120+H120+I120+J120+K120+L120+M120+N120+O120+O120)</f>
+        <v>4</v>
       </c>
       <c r="Q120" s="3">
         <f>ROUND(SUM(P120/2),0)</f>
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="T120" t="s">
         <v>137</v>
@@ -6754,111 +6746,121 @@
       </c>
     </row>
     <row r="121" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="40"/>
-      <c r="B121" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C121" s="14">
-        <v>111900</v>
-      </c>
-      <c r="D121" s="10">
-        <f>SUM(D119:D120)</f>
-        <v>0</v>
-      </c>
-      <c r="E121" s="10">
-        <f t="shared" ref="E121:P121" si="70">SUM(E119:E120)</f>
-        <v>0</v>
-      </c>
-      <c r="F121" s="10">
+      <c r="A121" s="35"/>
+      <c r="B121" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C121" s="13">
+        <v>112000</v>
+      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3">
+        <v>32</v>
+      </c>
+      <c r="I121" s="3">
+        <v>117</v>
+      </c>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3"/>
+      <c r="M121" s="3"/>
+      <c r="N121" s="3"/>
+      <c r="O121" s="3"/>
+      <c r="P121" s="3">
         <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="G121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="H121" s="10">
-        <f t="shared" si="70"/>
-        <v>34</v>
-      </c>
-      <c r="I121" s="10">
-        <f t="shared" si="70"/>
-        <v>119</v>
-      </c>
-      <c r="J121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="K121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="L121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="M121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="N121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="O121" s="10">
-        <f t="shared" si="70"/>
-        <v>0</v>
-      </c>
-      <c r="P121" s="10">
-        <f t="shared" si="70"/>
-        <v>153</v>
-      </c>
-      <c r="Q121" s="10">
-        <f>SUM(P121/2)</f>
-        <v>76.5</v>
+        <v>149</v>
+      </c>
+      <c r="Q121" s="3">
+        <f>ROUND(SUM(P121/2),0)</f>
+        <v>75</v>
       </c>
       <c r="T121" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A122" s="34" t="s">
+      <c r="U121" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="36"/>
+      <c r="B122" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" s="13">
+        <v>112100</v>
+      </c>
+      <c r="D122" s="10">
+        <f>SUM(D120:D121)</f>
+        <v>0</v>
+      </c>
+      <c r="E122" s="10">
+        <f t="shared" ref="E122:P122" si="71">SUM(E120:E121)</f>
+        <v>0</v>
+      </c>
+      <c r="F122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="G122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="H122" s="10">
+        <f t="shared" si="71"/>
+        <v>34</v>
+      </c>
+      <c r="I122" s="10">
+        <f t="shared" si="71"/>
+        <v>119</v>
+      </c>
+      <c r="J122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="K122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="L122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="M122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="N122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="O122" s="10">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="P122" s="10">
+        <f t="shared" si="71"/>
+        <v>153</v>
+      </c>
+      <c r="Q122" s="10">
+        <f>SUM(P122/2)</f>
+        <v>76.5</v>
+      </c>
+      <c r="T122" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A123" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="B123" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C122" s="14">
-        <v>112000</v>
-      </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
-      <c r="O122" s="3"/>
-      <c r="P122" s="3">
-        <f t="shared" ref="P122:P126" si="71">SUM(D122+E122+F122+G122+H122+I122+J122+K122+L122+M122+N122+O122+O122)</f>
-        <v>0</v>
-      </c>
-      <c r="Q122" s="3">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
-      <c r="B123" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C123" s="14">
-        <v>112100</v>
+      <c r="C123" s="13">
+        <v>112200</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
@@ -6873,34 +6875,28 @@
       <c r="N123" s="3"/>
       <c r="O123" s="3"/>
       <c r="P123" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" ref="P123:P127" si="72">SUM(D123+E123+F123+G123+H123+I123+J123+K123+L123+M123+N123+O123+O123)</f>
         <v>0</v>
       </c>
       <c r="Q123" s="3">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B124" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C124" s="14">
-        <v>112200</v>
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A124" s="32"/>
+      <c r="B124" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C124" s="13">
+        <v>112300</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
-      <c r="H124" s="3">
-        <v>1</v>
-      </c>
-      <c r="I124" s="3">
-        <v>5</v>
-      </c>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
@@ -6908,40 +6904,33 @@
       <c r="N124" s="3"/>
       <c r="O124" s="3"/>
       <c r="P124" s="3">
-        <f t="shared" si="71"/>
-        <v>6</v>
+        <f t="shared" si="72"/>
+        <v>0</v>
       </c>
       <c r="Q124" s="3">
-        <f>(AVERAGE(D124,E124,F124,G124,H124,I124,J124))</f>
-        <v>3</v>
-      </c>
-      <c r="T124" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="U124" s="36"/>
-      <c r="V124" s="36"/>
-      <c r="W124" s="36"/>
-      <c r="X124" s="36"/>
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B125" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C125" s="14">
-        <v>112300</v>
+      <c r="A125" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C125" s="13">
+        <v>112400</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I125" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
@@ -6950,38 +6939,40 @@
       <c r="N125" s="3"/>
       <c r="O125" s="3"/>
       <c r="P125" s="3">
-        <f t="shared" si="71"/>
-        <v>11</v>
+        <f t="shared" si="72"/>
+        <v>6</v>
       </c>
       <c r="Q125" s="3">
-        <f t="shared" ref="Q125:Q126" si="72">ROUND(SUM(P125/2),0)</f>
-        <v>6</v>
-      </c>
-      <c r="T125" s="36" t="s">
+        <f>(AVERAGE(D125,E125,F125,G125,H125,I125,J125))</f>
+        <v>3</v>
+      </c>
+      <c r="T125" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="U125" s="36"/>
-      <c r="V125" s="36"/>
-      <c r="W125" s="36"/>
-      <c r="X125" s="36"/>
+      <c r="U125" s="29"/>
+      <c r="V125" s="29"/>
+      <c r="W125" s="29"/>
+      <c r="X125" s="29"/>
     </row>
     <row r="126" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="24"/>
-      <c r="B126" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C126" s="14">
-        <v>112400</v>
+      <c r="A126" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B126" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C126" s="13">
+        <v>112500</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I126" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
@@ -6990,40 +6981,64 @@
       <c r="N126" s="3"/>
       <c r="O126" s="3"/>
       <c r="P126" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
+        <v>11</v>
+      </c>
+      <c r="Q126" s="3">
+        <f t="shared" ref="Q126" si="73">ROUND(SUM(P126/2),0)</f>
+        <v>6</v>
+      </c>
+      <c r="T126" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="U126" s="29"/>
+      <c r="V126" s="29"/>
+      <c r="W126" s="29"/>
+      <c r="X126" s="29"/>
+    </row>
+    <row r="127" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="23"/>
+      <c r="B127" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C127" s="13">
+        <v>112600</v>
+      </c>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3">
+        <v>11</v>
+      </c>
+      <c r="I127" s="3">
+        <v>6</v>
+      </c>
+      <c r="J127" s="3"/>
+      <c r="K127" s="3"/>
+      <c r="L127" s="3"/>
+      <c r="M127" s="3"/>
+      <c r="N127" s="3"/>
+      <c r="O127" s="3"/>
+      <c r="P127" s="3">
+        <f t="shared" si="72"/>
         <v>17</v>
       </c>
-      <c r="Q126" s="3">
-        <f>(AVERAGE(D124,E124,F124,G124,H124,I124,J124))</f>
+      <c r="Q127" s="3">
+        <f>(AVERAGE(D125,E125,F125,G125,H125,I125,J125))</f>
         <v>3</v>
       </c>
-      <c r="T126" s="36" t="s">
+      <c r="T127" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="U126" s="36"/>
-      <c r="V126" s="36"/>
-      <c r="W126" s="36"/>
-      <c r="X126" s="36"/>
+      <c r="U127" s="29"/>
+      <c r="V127" s="29"/>
+      <c r="W127" s="29"/>
+      <c r="X127" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="T124:X124"/>
-    <mergeCell ref="T125:X125"/>
-    <mergeCell ref="T126:X126"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A61"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A67:A76"/>
-    <mergeCell ref="A77:A85"/>
-    <mergeCell ref="A90:A94"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="A110:A115"/>
     <mergeCell ref="A48:A50"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
@@ -7035,6 +7050,22 @@
     <mergeCell ref="A24:A31"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A45:A47"/>
+    <mergeCell ref="T125:X125"/>
+    <mergeCell ref="T126:X126"/>
+    <mergeCell ref="T127:X127"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A61"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A122"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A67:A76"/>
+    <mergeCell ref="A77:A85"/>
+    <mergeCell ref="A90:A94"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A108:A109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7282,21 +7313,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7320,6 +7351,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D27F484E-3F35-4737-9237-6DDD4EEDE553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3298D6C9-3E24-4004-98FE-A66387B3B634}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -7337,14 +7376,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D27F484E-3F35-4737-9237-6DDD4EEDE553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72b17115-9915-42c0-9f1b-4f98e5a4bcd2}" enabled="0" method="" siteId="{72b17115-9915-42c0-9f1b-4f98e5a4bcd2}" removed="1"/>

</xml_diff>

<commit_message>
Removed Elevator from non monitor
Removed Elevator from non monitor
</commit_message>
<xml_diff>
--- a/Documentation/Metrics fields and sequence number.xlsx
+++ b/Documentation/Metrics fields and sequence number.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centurylink-my.sharepoint.com/personal/billy_bennett_lumen_com/Documents/Documents/GitHub/HSORehdMetrics/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{37FC37B3-BAA5-4352-A6BF-C4578865D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41D93BA0-2CD4-4CD9-B778-E88CE14CFBC3}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{37FC37B3-BAA5-4352-A6BF-C4578865D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3D1EE35-0095-4510-8CCB-065531B17CF3}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B754616-214D-4C02-8CFF-EFF6D36CED80}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="147">
   <si>
     <t>Category</t>
   </si>
@@ -126,9 +126,6 @@
     <t xml:space="preserve">Camera </t>
   </si>
   <si>
-    <t>Intercom</t>
-  </si>
-  <si>
     <t>CLEC Attrition</t>
   </si>
   <si>
@@ -472,6 +469,12 @@
   </si>
   <si>
     <t>Website views</t>
+  </si>
+  <si>
+    <t>Elevator</t>
+  </si>
+  <si>
+    <t>10/4/23 removed from Non Monitored and added to the Monitored totals</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +562,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -774,8 +783,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -785,6 +800,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -798,21 +819,13 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1130,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66A4A06-3F38-46D9-B8DB-D4324A9B592B}">
   <dimension ref="A1:X127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1213,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1241,7 +1254,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1280,7 +1293,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
@@ -1319,7 +1332,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1384,7 +1397,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1425,7 +1438,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1464,7 +1477,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1503,7 +1516,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1581,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1635,7 +1648,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -1700,7 +1713,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1765,7 +1778,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1830,7 +1843,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1871,7 +1884,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
@@ -1910,7 +1923,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="7" t="s">
         <v>13</v>
       </c>
@@ -1948,8 +1961,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
       <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
@@ -2013,8 +2026,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2054,8 +2067,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
@@ -2093,8 +2106,8 @@
         <v>6196</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
       <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
@@ -2132,8 +2145,8 @@
         <v>5495</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
@@ -2171,8 +2184,8 @@
         <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
       <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
@@ -2210,8 +2223,8 @@
         <v>583</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
       <c r="B23" s="7" t="s">
         <v>16</v>
       </c>
@@ -2275,8 +2288,8 @@
         <v>6395</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2316,8 +2329,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
       <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
@@ -2355,8 +2368,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
@@ -2394,8 +2407,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
@@ -2433,8 +2446,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
       <c r="B28" s="7" t="s">
         <v>28</v>
       </c>
@@ -2472,8 +2485,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
@@ -2511,49 +2524,52 @@
         <v>574</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="13">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
+      <c r="B30" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="42">
         <v>102800</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="43">
         <v>6</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="43">
         <v>6</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="43">
         <v>6</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="43">
         <v>6</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="43">
         <v>6</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3">
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43">
         <f t="shared" si="16"/>
         <v>30</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30" s="43">
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
+      <c r="T30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="13">
         <v>102900</v>
@@ -2615,8 +2631,8 @@
         <v>981</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -2657,7 +2673,7 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="7" t="s">
         <v>19</v>
       </c>
@@ -2696,7 +2712,7 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="7" t="s">
         <v>20</v>
       </c>
@@ -2735,7 +2751,7 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
@@ -2774,7 +2790,7 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="7" t="s">
         <v>22</v>
       </c>
@@ -2813,7 +2829,7 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -2854,7 +2870,7 @@
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="7" t="s">
         <v>19</v>
       </c>
@@ -2893,7 +2909,7 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="7" t="s">
         <v>20</v>
       </c>
@@ -2932,7 +2948,7 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="7" t="s">
         <v>21</v>
       </c>
@@ -2971,7 +2987,7 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="8" t="s">
         <v>22</v>
       </c>
@@ -3010,11 +3026,11 @@
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
-        <v>31</v>
+      <c r="A42" s="32" t="s">
+        <v>30</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="13">
         <v>104000</v>
@@ -3078,9 +3094,9 @@
       <c r="S42" s="12"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="13">
         <v>104100</v>
@@ -3143,9 +3159,9 @@
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="32"/>
       <c r="B44" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="13">
         <v>104200</v>
@@ -3207,15 +3223,15 @@
         <v>-4.9135577797998183E-3</v>
       </c>
       <c r="T44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
-        <v>32</v>
+      <c r="A45" s="32" t="s">
+        <v>31</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="13">
         <v>104300</v>
@@ -3278,9 +3294,9 @@
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="13">
         <v>104400</v>
@@ -3343,9 +3359,9 @@
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="13">
         <v>104500</v>
@@ -3407,15 +3423,15 @@
         <v>-1.2618296529968454E-2</v>
       </c>
       <c r="T47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
-        <v>33</v>
+      <c r="A48" s="32" t="s">
+        <v>32</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="13">
         <v>104600</v>
@@ -3479,9 +3495,9 @@
       <c r="S48" s="12"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="13">
         <v>104700</v>
@@ -3544,9 +3560,9 @@
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="13">
         <v>104800</v>
@@ -3608,15 +3624,15 @@
         <v>-1.7152658662092624E-3</v>
       </c>
       <c r="T50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C51" s="13">
         <v>104900</v>
@@ -3679,9 +3695,9 @@
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C52" s="13">
         <v>105000</v>
@@ -3744,9 +3760,9 @@
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C53" s="13">
         <v>105100</v>
@@ -3808,15 +3824,15 @@
         <v>-4.8475371383893667E-3</v>
       </c>
       <c r="T53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="C54" s="13">
         <v>105200</v>
@@ -3853,9 +3869,9 @@
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="32"/>
+      <c r="A55" s="34"/>
       <c r="B55" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C55" s="13">
         <v>105300</v>
@@ -3892,9 +3908,9 @@
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+      <c r="A56" s="34"/>
       <c r="B56" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" s="15">
         <v>105400</v>
@@ -3931,9 +3947,9 @@
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
+      <c r="A57" s="34"/>
       <c r="B57" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C57" s="13">
         <v>105500</v>
@@ -3970,9 +3986,9 @@
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
+      <c r="A58" s="34"/>
       <c r="B58" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C58" s="13">
         <v>105600</v>
@@ -4009,9 +4025,9 @@
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
+      <c r="A59" s="34"/>
       <c r="B59" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C59" s="13">
         <v>105700</v>
@@ -4048,9 +4064,9 @@
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+      <c r="A60" s="34"/>
       <c r="B60" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="13">
         <v>105800</v>
@@ -4087,9 +4103,9 @@
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
+      <c r="A61" s="34"/>
       <c r="B61" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" s="13">
         <v>105900</v>
@@ -4126,11 +4142,11 @@
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="C62" s="13">
         <v>106000</v>
@@ -4167,9 +4183,9 @@
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
+      <c r="A63" s="34"/>
       <c r="B63" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C63" s="13">
         <v>106100</v>
@@ -4206,9 +4222,9 @@
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
+      <c r="A64" s="34"/>
       <c r="B64" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" s="13">
         <v>106200</v>
@@ -4245,9 +4261,9 @@
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" s="13">
         <v>106300</v>
@@ -4284,9 +4300,9 @@
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="37"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C66" s="13">
         <v>106400</v>
@@ -4349,11 +4365,11 @@
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="s">
+      <c r="A67" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="C67" s="13">
         <v>106500</v>
@@ -4390,9 +4406,9 @@
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68" s="13">
         <v>106600</v>
@@ -4429,9 +4445,9 @@
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" s="13">
         <v>106700</v>
@@ -4468,9 +4484,9 @@
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="32"/>
       <c r="B70" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" s="13">
         <v>106800</v>
@@ -4507,9 +4523,9 @@
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" s="13">
         <v>106900</v>
@@ -4546,9 +4562,9 @@
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="32"/>
       <c r="B72" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C72" s="13">
         <v>107000</v>
@@ -4611,9 +4627,9 @@
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" s="13">
         <v>107100</v>
@@ -4650,9 +4666,9 @@
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="32"/>
       <c r="B74" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C74" s="13">
         <v>107200</v>
@@ -4715,13 +4731,13 @@
       </c>
       <c r="S74" s="12"/>
       <c r="T74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
+      <c r="A75" s="32"/>
       <c r="B75" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75" s="13">
         <v>107300</v>
@@ -4758,9 +4774,9 @@
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="32"/>
       <c r="B76" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C76" s="13">
         <v>107400</v>
@@ -4822,15 +4838,15 @@
         <v>0</v>
       </c>
       <c r="T76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="C77" s="13">
         <v>107500</v>
@@ -4867,9 +4883,9 @@
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78" s="13">
         <v>107600</v>
@@ -4906,9 +4922,9 @@
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A79" s="30"/>
+      <c r="A79" s="32"/>
       <c r="B79" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C79" s="13">
         <v>107700</v>
@@ -4971,9 +4987,9 @@
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="32"/>
       <c r="B80" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80" s="13">
         <v>107800</v>
@@ -5010,9 +5026,9 @@
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
+      <c r="A81" s="32"/>
       <c r="B81" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81" s="13">
         <v>107900</v>
@@ -5049,9 +5065,9 @@
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="32"/>
       <c r="B82" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C82" s="13">
         <v>108000</v>
@@ -5088,9 +5104,9 @@
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A83" s="30"/>
+      <c r="A83" s="32"/>
       <c r="B83" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C83" s="13">
         <v>108100</v>
@@ -5127,9 +5143,9 @@
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="32"/>
       <c r="B84" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C84" s="13">
         <v>108200</v>
@@ -5191,13 +5207,13 @@
         <v>0</v>
       </c>
       <c r="T84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="32"/>
       <c r="B85" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C85" s="13">
         <v>108300</v>
@@ -5230,11 +5246,11 @@
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="31" t="s">
-        <v>94</v>
+      <c r="A86" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C86" s="13">
         <v>108400</v>
@@ -5267,9 +5283,9 @@
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A87" s="32"/>
+      <c r="A87" s="34"/>
       <c r="B87" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C87" s="13">
         <v>108500</v>
@@ -5302,9 +5318,9 @@
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A88" s="32"/>
+      <c r="A88" s="34"/>
       <c r="B88" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C88" s="13">
         <v>108600</v>
@@ -5337,9 +5353,9 @@
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A89" s="37"/>
+      <c r="A89" s="35"/>
       <c r="B89" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C89" s="13">
         <v>108700</v>
@@ -5402,11 +5418,11 @@
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A90" s="38" t="s">
-        <v>83</v>
+      <c r="A90" s="41" t="s">
+        <v>82</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" s="13">
         <v>108800</v>
@@ -5443,9 +5459,9 @@
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A91" s="38"/>
+      <c r="A91" s="41"/>
       <c r="B91" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C91" s="13">
         <v>108900</v>
@@ -5482,9 +5498,9 @@
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A92" s="38"/>
+      <c r="A92" s="41"/>
       <c r="B92" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C92" s="13">
         <v>109000</v>
@@ -5546,14 +5562,14 @@
         <v>5.7279236276849645E-2</v>
       </c>
       <c r="T92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V92" s="24"/>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A93" s="39"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C93" s="13">
         <v>109100</v>
@@ -5588,13 +5604,13 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="T93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A94" s="39"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C94" s="13">
         <v>109200</v>
@@ -5630,13 +5646,13 @@
         <v>10</v>
       </c>
       <c r="T94" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>
       <c r="B95" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C95" s="13">
         <v>109300</v>
@@ -5675,7 +5691,7 @@
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
       <c r="B96" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C96" s="13">
         <v>109400</v>
@@ -5714,7 +5730,7 @@
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="16"/>
       <c r="B97" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C97" s="13">
         <v>109500</v>
@@ -5776,13 +5792,13 @@
         <v>0.20930232558139536</v>
       </c>
       <c r="T97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
       <c r="B98" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C98" s="13">
         <v>109600</v>
@@ -5817,13 +5833,13 @@
         <v>4.9660000000000002</v>
       </c>
       <c r="T98" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
       <c r="B99" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C99" s="13">
         <v>109700</v>
@@ -5858,15 +5874,15 @@
         <v>9.7729999999999997</v>
       </c>
       <c r="T99" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="C100" s="13">
         <v>109800</v>
@@ -5887,11 +5903,11 @@
       <c r="Q100" s="3"/>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A101" s="39" t="s">
+      <c r="A101" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B101" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="C101" s="13">
         <v>110000</v>
@@ -5928,9 +5944,9 @@
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A102" s="40"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C102" s="13">
         <v>110100</v>
@@ -5959,13 +5975,13 @@
         <v>98.81</v>
       </c>
       <c r="T102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="41"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C103" s="13">
         <v>110200</v>
@@ -5975,7 +5991,7 @@
       </c>
       <c r="E103" s="27"/>
       <c r="F103" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G103" s="27">
         <v>52.54</v>
@@ -5996,15 +6012,15 @@
         <v>75.44</v>
       </c>
       <c r="T103" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="s">
-        <v>86</v>
+      <c r="A104" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C104" s="13">
         <v>110300</v>
@@ -6041,9 +6057,9 @@
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="32"/>
       <c r="B105" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C105" s="13">
         <v>110400</v>
@@ -6079,13 +6095,13 @@
         <v>3</v>
       </c>
       <c r="T105" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="32"/>
       <c r="B106" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C106" s="13">
         <v>110500</v>
@@ -6122,9 +6138,9 @@
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A107" s="30"/>
+      <c r="A107" s="32"/>
       <c r="B107" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C107" s="13">
         <v>110600</v>
@@ -6187,11 +6203,11 @@
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A108" s="31" t="s">
-        <v>101</v>
+      <c r="A108" s="33" t="s">
+        <v>100</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C108" s="13">
         <v>110700</v>
@@ -6228,9 +6244,9 @@
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A109" s="37"/>
+      <c r="A109" s="35"/>
       <c r="B109" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C109" s="13">
         <v>110800</v>
@@ -6266,15 +6282,15 @@
         <v>5</v>
       </c>
       <c r="T109" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A110" s="39" t="s">
+      <c r="A110" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B110" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="C110" s="13">
         <v>110900</v>
@@ -6311,9 +6327,9 @@
       </c>
     </row>
     <row r="111" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="40"/>
+      <c r="A111" s="30"/>
       <c r="B111" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C111" s="13">
         <v>111000</v>
@@ -6349,13 +6365,13 @@
         <v>5341</v>
       </c>
       <c r="T111" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="40"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C112" s="13">
         <v>111100</v>
@@ -6391,13 +6407,13 @@
         <v>17400</v>
       </c>
       <c r="T112" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="40"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C113" s="13">
         <v>111200</v>
@@ -6433,13 +6449,13 @@
         <v>3200</v>
       </c>
       <c r="T113" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="40"/>
+      <c r="A114" s="30"/>
       <c r="B114" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C114" s="13">
         <v>111300</v>
@@ -6475,13 +6491,13 @@
         <v>12200</v>
       </c>
       <c r="T114" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="41"/>
+      <c r="A115" s="31"/>
       <c r="B115" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C115" s="13">
         <v>111400</v>
@@ -6517,15 +6533,15 @@
         <v>143173</v>
       </c>
       <c r="T115" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A116" s="31" t="s">
-        <v>95</v>
+      <c r="A116" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C116" s="13">
         <v>111500</v>
@@ -6562,9 +6578,9 @@
       </c>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A117" s="32"/>
+      <c r="A117" s="34"/>
       <c r="B117" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C117" s="13">
         <v>111600</v>
@@ -6601,9 +6617,9 @@
       </c>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A118" s="32"/>
+      <c r="A118" s="34"/>
       <c r="B118" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C118" s="13">
         <v>111700</v>
@@ -6666,9 +6682,9 @@
       </c>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A119" s="33"/>
+      <c r="A119" s="37"/>
       <c r="B119" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C119" s="13">
         <v>111800</v>
@@ -6705,11 +6721,11 @@
       </c>
     </row>
     <row r="120" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="34" t="s">
+      <c r="A120" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B120" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="B120" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="C120" s="13">
         <v>111900</v>
@@ -6739,16 +6755,16 @@
         <v>2</v>
       </c>
       <c r="T120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U120" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="35"/>
+      <c r="A121" s="39"/>
       <c r="B121" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C121" s="13">
         <v>112000</v>
@@ -6778,16 +6794,16 @@
         <v>75</v>
       </c>
       <c r="T121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U121" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="36"/>
+      <c r="A122" s="40"/>
       <c r="B122" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C122" s="13">
         <v>112100</v>
@@ -6849,15 +6865,15 @@
         <v>76.5</v>
       </c>
       <c r="T122" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A123" s="32" t="s">
-        <v>95</v>
+      <c r="A123" s="34" t="s">
+        <v>94</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C123" s="13">
         <v>112200</v>
@@ -6884,9 +6900,9 @@
       </c>
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A124" s="32"/>
+      <c r="A124" s="34"/>
       <c r="B124" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C124" s="13">
         <v>112300</v>
@@ -6914,10 +6930,10 @@
     </row>
     <row r="125" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B125" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="B125" s="20" t="s">
-        <v>131</v>
       </c>
       <c r="C125" s="13">
         <v>112400</v>
@@ -6946,20 +6962,20 @@
         <f>(AVERAGE(D125,E125,F125,G125,H125,I125,J125))</f>
         <v>3</v>
       </c>
-      <c r="T125" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="U125" s="29"/>
-      <c r="V125" s="29"/>
-      <c r="W125" s="29"/>
-      <c r="X125" s="29"/>
+      <c r="T125" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="U125" s="36"/>
+      <c r="V125" s="36"/>
+      <c r="W125" s="36"/>
+      <c r="X125" s="36"/>
     </row>
     <row r="126" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B126" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C126" s="13">
         <v>112500</v>
@@ -6988,18 +7004,18 @@
         <f t="shared" ref="Q126" si="73">ROUND(SUM(P126/2),0)</f>
         <v>6</v>
       </c>
-      <c r="T126" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="U126" s="29"/>
-      <c r="V126" s="29"/>
-      <c r="W126" s="29"/>
-      <c r="X126" s="29"/>
+      <c r="T126" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="U126" s="36"/>
+      <c r="V126" s="36"/>
+      <c r="W126" s="36"/>
+      <c r="X126" s="36"/>
     </row>
     <row r="127" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="23"/>
       <c r="B127" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C127" s="13">
         <v>112600</v>
@@ -7028,28 +7044,16 @@
         <f>(AVERAGE(D125,E125,F125,G125,H125,I125,J125))</f>
         <v>3</v>
       </c>
-      <c r="T127" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="U127" s="29"/>
-      <c r="V127" s="29"/>
-      <c r="W127" s="29"/>
-      <c r="X127" s="29"/>
+      <c r="T127" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="U127" s="36"/>
+      <c r="V127" s="36"/>
+      <c r="W127" s="36"/>
+      <c r="X127" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A110:A115"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
     <mergeCell ref="T125:X125"/>
     <mergeCell ref="T126:X126"/>
     <mergeCell ref="T127:X127"/>
@@ -7066,6 +7070,18 @@
     <mergeCell ref="A86:A89"/>
     <mergeCell ref="A101:A103"/>
     <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A110:A115"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7073,6 +7089,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010048F37C2ACA71DA4BBEA1AF332FC548D0" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eac57c200053c00c3fb94f7d74e7e878">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="51b4bdac-ea34-4e29-8b01-203f27abe1e9" xmlns:ns4="53225991-f7ab-4c8a-bafc-653fbe8e73f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c7226b8f5adfb3952019efb9affd493" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7312,15 +7337,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7331,6 +7347,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D27F484E-3F35-4737-9237-6DDD4EEDE553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{431E5728-E87E-4E55-9342-116574452738}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7346,14 +7370,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D27F484E-3F35-4737-9237-6DDD4EEDE553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>